<commit_message>
changing latest payment date to payment date
</commit_message>
<xml_diff>
--- a/test/complex_test_case_1.xlsx
+++ b/test/complex_test_case_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/limnaroline/forecasting-project/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C33AB10D-0CF2-6444-9D05-79EA9D63621F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED96B557-4AF1-2B4C-A6E6-5D85EF3F3769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13580" yWindow="1520" windowWidth="20500" windowHeight="13600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>Planned Amount</t>
   </si>
   <si>
-    <t>Latest Payment Date</t>
-  </si>
-  <si>
     <t>trip to sydney</t>
   </si>
   <si>
@@ -114,6 +111,9 @@
   </si>
   <si>
     <t>amy's salary</t>
+  </si>
+  <si>
+    <t>Payment Date</t>
   </si>
 </sst>
 </file>
@@ -495,10 +495,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1">
         <v>45658</v>
@@ -512,10 +512,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1">
         <v>45839</v>
@@ -529,10 +529,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1">
         <v>45658</v>
@@ -546,10 +546,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
       </c>
       <c r="C5" s="1">
         <v>45658</v>
@@ -563,10 +563,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1">
         <v>45658</v>
@@ -589,7 +589,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -612,7 +612,7 @@
         <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -623,10 +623,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2">
         <v>20100</v>
@@ -640,10 +640,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="2">
         <v>4000</v>
@@ -657,10 +657,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="2">
         <v>4000</v>
@@ -674,10 +674,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2">
         <v>2500</v>
@@ -691,10 +691,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="2">
         <v>5000</v>
@@ -708,10 +708,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="2">
         <v>1000</v>
@@ -725,10 +725,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2">
         <v>1000</v>
@@ -742,10 +742,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="2">
         <v>500</v>

</xml_diff>